<commit_message>
V1.7 Output to Excel
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -427,157 +427,127 @@
           <t>Slot</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" t="n">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Pole</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Phase number</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Slots per phase</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Coil span</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Electrical angle per slot</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Slots per phase per pole</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Slot</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
         <is>
           <t>Phase A</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C8" t="inlineStr">
         <is>
           <t>Phase B</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="D8" t="inlineStr">
         <is>
           <t>Phase C</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>In</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Out &amp; Out</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>In</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>In</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Out &amp; Out</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>4</v>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>In</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>5</v>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>In</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>In</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>Out &amp; Out</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Out &amp; Out</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>In</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>In</t>
+          <t>In &amp; In</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>9</v>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>In</t>
+        <v>2</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Out &amp; Out</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Out &amp; Out</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>In</t>
+          <t>In &amp; In</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>11</v>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>In</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
+        <v>4</v>
+      </c>
+      <c r="B12" t="inlineStr">
         <is>
           <t>Out &amp; Out</t>
         </is>
@@ -585,11 +555,441 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
+        <v>5</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>In &amp; In</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>6</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Out &amp; Out</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>7</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>In &amp; In</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>8</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Out &amp; Out</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>9</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>In &amp; In</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>10</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Out &amp; Out</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>11</v>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>In &amp; In</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
         <v>12</v>
       </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>In</t>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Out &amp; Out</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>13</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>In &amp; In</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>14</v>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Out &amp; Out</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>15</v>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>In &amp; In</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>16</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Out &amp; Out</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>17</v>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>In &amp; In</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>18</v>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Out &amp; Out</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>19</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>In &amp; In</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>20</v>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Out &amp; Out</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>21</v>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>In &amp; In</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>22</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Out &amp; Out</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>23</v>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>In &amp; In</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>24</v>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Out &amp; Out</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>25</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>In &amp; In</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>26</v>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>Out &amp; Out</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>27</v>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>In &amp; In</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>28</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Out &amp; Out</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>29</v>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>In &amp; In</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>30</v>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Out &amp; Out</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>31</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>In &amp; In</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>32</v>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>Out &amp; Out</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>33</v>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>In &amp; In</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>34</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Out &amp; Out</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>35</v>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>In &amp; In</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>36</v>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Out &amp; Out</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>37</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>In &amp; In</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>38</v>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>Out &amp; Out</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>39</v>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>In &amp; In</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>40</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Out &amp; Out</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>41</v>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>In &amp; In</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>42</v>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Out &amp; Out</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>43</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>In &amp; In</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>44</v>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>Out &amp; Out</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>45</v>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>In &amp; In</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>46</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Out &amp; Out</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>47</v>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>In &amp; In</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>48</v>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Out &amp; Out</t>
         </is>
       </c>
     </row>

</xml_diff>